<commit_message>
Revert "Merge branch 'wrong-xlsform-col'"
This reverts commit 2a6d64a8faa80e087f8657aec6f148234f4bd715.
</commit_message>
<xml_diff>
--- a/spec/fixtures/files/decimal.xlsx
+++ b/spec/fixtures/files/decimal.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t xml:space="preserve">type</t>
   </si>
@@ -29,19 +29,22 @@
     <t xml:space="preserve">name</t>
   </si>
   <si>
+    <t xml:space="preserve">message</t>
+  </si>
+  <si>
+    <t xml:space="preserve">decimal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wine_temp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At what temperature do you like your red wine?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">list name</t>
+  </si>
+  <si>
     <t xml:space="preserve">label</t>
-  </si>
-  <si>
-    <t xml:space="preserve">decimal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wine_temp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">At what temperature do you like your red wine?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">list name</t>
   </si>
 </sst>
 </file>
@@ -56,7 +59,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -78,7 +80,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -152,7 +153,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="83" zoomScaleNormal="83" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -209,7 +210,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.63"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="11.52"/>
   </cols>
   <sheetData>
@@ -221,13 +222,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>